<commit_message>
Debug on the weights series, figure out how the weights is passed each day, need to modify the logic of which stock list to iterate
</commit_message>
<xml_diff>
--- a/牧鑫资产 暑期模拟盘.xlsx
+++ b/牧鑫资产 暑期模拟盘.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="12">
   <si>
     <t>交易日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,13 +65,22 @@
     <t>总市值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>总收益率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当日盈亏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -112,7 +121,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -123,6 +132,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -405,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:H130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -416,9 +428,10 @@
     <col min="1" max="1" width="10.5" customWidth="1"/>
     <col min="3" max="4" width="12.75" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
+    <col min="7" max="7" width="11.625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +447,14 @@
       <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>45483</v>
       </c>
@@ -452,8 +471,16 @@
         <f>C2/D2</f>
         <v>0.18837977040166282</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G2" s="4">
+        <f>D2-1000000</f>
+        <v>165.78000000002794</v>
+      </c>
+      <c r="H2" s="3">
+        <f>D2/1000000-1</f>
+        <v>1.6578000000011528E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -467,8 +494,16 @@
         <f t="shared" ref="E3:E23" si="0">C3/D3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G6" si="1">D3-1000000</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <f>D3/1000000-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -482,8 +517,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G4" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <f>D4/1000000-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -497,8 +540,16 @@
         <f t="shared" si="0"/>
         <v>0.37527079652727519</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G5" s="4">
+        <f t="shared" si="1"/>
+        <v>-804.20999999996275</v>
+      </c>
+      <c r="H5" s="3">
+        <f>D5/1000000-1</f>
+        <v>-8.0420999999997189E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -512,8 +563,16 @@
         <f t="shared" si="0"/>
         <v>0.99956822475863749</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
+        <v>1053.2299999999814</v>
+      </c>
+      <c r="H6" s="3">
+        <f>D6/1000000-1</f>
+        <v>1.0532299999999051E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>45484</v>
       </c>
@@ -530,8 +589,16 @@
         <f>C7/D7</f>
         <v>0.50822342383961561</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G7" s="4">
+        <f>D7-D2</f>
+        <v>4221.2199999999721</v>
+      </c>
+      <c r="H7" s="3">
+        <f>D7/1000000-1</f>
+        <v>4.3869999999999187E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -545,8 +612,16 @@
         <f>C8/D8</f>
         <v>0.27049476048787746</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G8" s="4">
+        <f t="shared" ref="G8:G21" si="2">D8-D3</f>
+        <v>1331.7800000000279</v>
+      </c>
+      <c r="H8" s="3">
+        <f>D8/1000000-1</f>
+        <v>1.3317800000001156E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -560,8 +635,16 @@
         <f t="shared" si="0"/>
         <v>0.99920885265634007</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G9" s="4">
+        <f t="shared" si="2"/>
+        <v>6601.3699999999953</v>
+      </c>
+      <c r="H9" s="3">
+        <f>D9/1000000-1</f>
+        <v>6.6013700000000508E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -575,8 +658,16 @@
         <f t="shared" si="0"/>
         <v>0.38280013524795986</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G10" s="4">
+        <f t="shared" si="2"/>
+        <v>12191</v>
+      </c>
+      <c r="H10" s="3">
+        <f>D10/1000000-1</f>
+        <v>1.138678999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -590,165 +681,305 @@
         <f t="shared" si="0"/>
         <v>0.99957370329558037</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G11" s="4">
+        <f t="shared" si="2"/>
+        <v>12865</v>
+      </c>
+      <c r="H11" s="3">
+        <f>D11/1000000-1</f>
+        <v>1.3918230000000031E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>45485</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C12" s="2">
+        <v>880967</v>
+      </c>
+      <c r="D12" s="2">
+        <v>978544.21</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.9002832891934438</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="2"/>
+        <v>-25842.790000000037</v>
+      </c>
+      <c r="H12" s="3">
+        <f>D12/1000000-1</f>
+        <v>-2.1455790000000086E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C13" s="2">
+        <v>369835</v>
+      </c>
+      <c r="D13" s="2">
+        <v>998039.07</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.37056164544740722</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="2"/>
+        <v>-3292.7100000000792</v>
+      </c>
+      <c r="H13" s="3">
+        <f>D13/1000000-1</f>
+        <v>-1.9609300000000829E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C14" s="2">
+        <v>998246</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1000596.44</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99765096106078499</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="2"/>
+        <v>-6004.9300000000512</v>
+      </c>
+      <c r="H14" s="3">
+        <f>D14/1000000-1</f>
+        <v>5.9644000000003139E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C15" s="2">
+        <v>461722</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1013925.75</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.45538048520811314</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="2"/>
+        <v>2538.9599999999627</v>
+      </c>
+      <c r="H15" s="3">
+        <f>D15/1000000-1</f>
+        <v>1.392575000000007E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C16" s="2">
+        <v>1012099</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1012531.23</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99957311933973636</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="2"/>
+        <v>-1387</v>
+      </c>
+      <c r="H16" s="3">
+        <f>D16/1000000-1</f>
+        <v>1.2531230000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>45488</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C17" s="2">
+        <v>886708</v>
+      </c>
+      <c r="D17" s="2">
+        <v>987437.21</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.897989250374715</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="2"/>
+        <v>8893</v>
+      </c>
+      <c r="H17" s="3">
+        <f>D17/1000000-1</f>
+        <v>-1.2562790000000046E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C18" s="2">
+        <v>851615</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1002004.37</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>0.84991146296098485</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="2"/>
+        <v>3965.3000000000466</v>
+      </c>
+      <c r="H18" s="3">
+        <f>D18/1000000-1</f>
+        <v>2.0043700000000886E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C19" s="2">
+        <v>966151</v>
+      </c>
+      <c r="D19" s="2">
+        <v>968440.05</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99763635343251234</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="2"/>
+        <v>-32156.389999999898</v>
+      </c>
+      <c r="H19" s="3">
+        <f>D19/1000000-1</f>
+        <v>-3.1559950000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C20" s="2">
+        <v>465150</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1017353.75</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.45721559487051577</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="2"/>
+        <v>3428</v>
+      </c>
+      <c r="H20" s="3">
+        <f>D20/1000000-1</f>
+        <v>1.7353750000000057E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C21" s="2">
+        <v>1018046</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1018478.23</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99957561194017863</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="2"/>
+        <v>5947</v>
+      </c>
+      <c r="H21" s="3">
+        <f>D21/1000000-1</f>
+        <v>1.8478229999999929E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>45489</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>3</v>
       </c>

</xml_diff>